<commit_message>
Table 1 % vs proportion
</commit_message>
<xml_diff>
--- a/results/Table1_Antibiogram.xlsx
+++ b/results/Table1_Antibiogram.xlsx
@@ -248,85 +248,85 @@
     <t>GP</t>
   </si>
   <si>
-    <t>0.025 (1035)</t>
-  </si>
-  <si>
-    <t>0.17 (110)</t>
-  </si>
-  <si>
-    <t>0.39 (1091)</t>
-  </si>
-  <si>
-    <t>0.85 (943)</t>
-  </si>
-  <si>
-    <t>0.39 (800)</t>
-  </si>
-  <si>
-    <t>0.38 (1090)</t>
-  </si>
-  <si>
-    <t>0.36 (1028)</t>
-  </si>
-  <si>
-    <t>0.62 (144)</t>
-  </si>
-  <si>
-    <t>0.55 (56)</t>
-  </si>
-  <si>
-    <t>0.58 (1089)</t>
-  </si>
-  <si>
-    <t>0.15 (537)</t>
-  </si>
-  <si>
-    <t>0.16 (1085)</t>
-  </si>
-  <si>
-    <t>0.0019 (1030)</t>
-  </si>
-  <si>
-    <t>0.097 (1091)</t>
-  </si>
-  <si>
-    <t>0.036 (1091)</t>
-  </si>
-  <si>
-    <t>0.0087 (923)</t>
-  </si>
-  <si>
-    <t>0.0034 (290)</t>
-  </si>
-  <si>
-    <t>0.022 (458)</t>
-  </si>
-  <si>
-    <t>0.065 (1078)</t>
-  </si>
-  <si>
-    <t>0 (1088)</t>
-  </si>
-  <si>
-    <t>0.025 (1091)</t>
-  </si>
-  <si>
-    <t>0 (1091)</t>
-  </si>
-  <si>
-    <t>0.007 (718)</t>
-  </si>
-  <si>
-    <t>0.00092 (1091)</t>
-  </si>
-  <si>
-    <t>0 (390)</t>
-  </si>
-  <si>
-    <t>0.0029 (345)</t>
-  </si>
-  <si>
-    <t>0 (1090)</t>
+    <t>2.5% (1035)</t>
+  </si>
+  <si>
+    <t>17% (110)</t>
+  </si>
+  <si>
+    <t>39% (1091)</t>
+  </si>
+  <si>
+    <t>85% (943)</t>
+  </si>
+  <si>
+    <t>39% (800)</t>
+  </si>
+  <si>
+    <t>38% (1090)</t>
+  </si>
+  <si>
+    <t>36% (1028)</t>
+  </si>
+  <si>
+    <t>62% (144)</t>
+  </si>
+  <si>
+    <t>55% (56)</t>
+  </si>
+  <si>
+    <t>58% (1089)</t>
+  </si>
+  <si>
+    <t>15% (537)</t>
+  </si>
+  <si>
+    <t>16% (1085)</t>
+  </si>
+  <si>
+    <t>0.19% (1030)</t>
+  </si>
+  <si>
+    <t>9.7% (1091)</t>
+  </si>
+  <si>
+    <t>3.6% (1091)</t>
+  </si>
+  <si>
+    <t>0.87% (923)</t>
+  </si>
+  <si>
+    <t>0.34% (290)</t>
+  </si>
+  <si>
+    <t>2.2% (458)</t>
+  </si>
+  <si>
+    <t>6.5% (1078)</t>
+  </si>
+  <si>
+    <t>0% (1088)</t>
+  </si>
+  <si>
+    <t>2.5% (1091)</t>
+  </si>
+  <si>
+    <t>0% (1091)</t>
+  </si>
+  <si>
+    <t>0.7% (718)</t>
+  </si>
+  <si>
+    <t>0.092% (1091)</t>
+  </si>
+  <si>
+    <t>0% (390)</t>
+  </si>
+  <si>
+    <t>0.29% (345)</t>
+  </si>
+  <si>
+    <t>0% (1090)</t>
   </si>
 </sst>
 </file>

</xml_diff>